<commit_message>
Rendu du projet V2.0.2
Rendu des fichiers de fabrications, des rapports ainsi que de toute l'arborescence complète
</commit_message>
<xml_diff>
--- a/rpt/Journal de travail/carte_electronique_didactique_PittetL02-rpt-journal.xlsx
+++ b/rpt/Journal de travail/carte_electronique_didactique_PittetL02-rpt-journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/loic_pittet_studentfr_ch/Documents/TPI_PITTETL02/tpi_carte_electronique_didactique_pittetl02/rpt/Journal de travail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="944" documentId="11_416AEE08F1E9306E2D9B4F0BC9E4841233F83705" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96380422-9E6E-4057-A731-CC71698D8BEC}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="11_416AEE08F1E9306E2D9B4F0BC9E4841233F83705" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0662815E-7331-47E8-8811-497838C45343}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="15" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="154">
   <si>
     <t>Date</t>
   </si>
@@ -118,21 +118,6 @@
     <t>Pittet Loïc</t>
   </si>
   <si>
-    <t>[2024-09-16]</t>
-  </si>
-  <si>
-    <t>[2024-09-17]</t>
-  </si>
-  <si>
-    <t>[2024-09-18]</t>
-  </si>
-  <si>
-    <t>[2024-09-19]</t>
-  </si>
-  <si>
-    <t>[2024-09-20]</t>
-  </si>
-  <si>
     <t>[2024-09-23]</t>
   </si>
   <si>
@@ -163,9 +148,6 @@
     <t>[2024-09-30]</t>
   </si>
   <si>
-    <t>Altium</t>
-  </si>
-  <si>
     <t>Production</t>
   </si>
   <si>
@@ -196,18 +178,9 @@
     <t>[2024-10-28]</t>
   </si>
   <si>
-    <t>Présentation</t>
-  </si>
-  <si>
-    <t>Divers</t>
-  </si>
-  <si>
     <t>Programmation</t>
   </si>
   <si>
-    <t>Absent</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -524,6 +497,27 @@
   </si>
   <si>
     <t>[2025-05-26]</t>
+  </si>
+  <si>
+    <t>Modifications dernières erreures pour pouvoir commander une nouvelle version pour la présentation</t>
+  </si>
+  <si>
+    <t>[2025-06-02]</t>
+  </si>
+  <si>
+    <t>[2025-06-03]</t>
+  </si>
+  <si>
+    <t>[2025-06-04]</t>
+  </si>
+  <si>
+    <t>Remplissage rpt de travail, de développement et de l'arboréscence</t>
+  </si>
+  <si>
+    <t>Fin du projet. J'ai réussi à le mener au bout. Cette dernière semaine a été très documentative. J'ai mis à jour toute l'arboréscence avec l'ajout de toutes mes prises de notes. J'ai terminé mon rapport de développement ainsi que de travail. J'ai fait en sorte de rendre tous les documents.</t>
+  </si>
+  <si>
+    <t>Recherches</t>
   </si>
 </sst>
 </file>
@@ -1246,6 +1240,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>Graphique</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CH" baseline="0"/>
+              <a:t> des heures effectués</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1538,10 +1562,10 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Divers</c:v>
+                  <c:v>Discussion</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Altium</c:v>
+                  <c:v>PCB</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Programmation</c:v>
@@ -1550,16 +1574,16 @@
                   <c:v>Production</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Mesures</c:v>
+                  <c:v>Tests</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Documentation</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Absent</c:v>
+                  <c:v>Schematic</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Présentation</c:v>
+                  <c:v>Recherches</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1570,6 +1594,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2576,57 +2624,84 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B4:B12"/>
+  <dimension ref="B4:C12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C4">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2640,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -2697,7 +2772,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>2</v>
@@ -2724,13 +2799,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="13">
@@ -2742,10 +2817,10 @@
       <c r="A6" s="43"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="13">
@@ -2757,10 +2832,10 @@
       <c r="A7" s="43"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="13">
@@ -2772,13 +2847,13 @@
       <c r="A8" s="43"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F8" s="6">
         <v>2</v>
@@ -2789,13 +2864,13 @@
       <c r="A9" s="43"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
@@ -2806,10 +2881,10 @@
       <c r="A10" s="43"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="6">
@@ -2819,7 +2894,7 @@
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2838,16 +2913,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="F12" s="6">
         <v>3</v>
@@ -2858,13 +2933,13 @@
       <c r="A13" s="43"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F13" s="6">
         <v>3</v>
@@ -2875,10 +2950,10 @@
       <c r="A14" s="43"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6">
@@ -2890,10 +2965,10 @@
       <c r="A15" s="43"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6">
@@ -2903,7 +2978,7 @@
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -2922,16 +2997,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F17" s="6">
         <v>0.5</v>
@@ -2942,10 +3017,10 @@
       <c r="A18" s="43"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="6">
@@ -2957,13 +3032,13 @@
       <c r="A19" s="43"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F19" s="6">
         <v>3</v>
@@ -2974,13 +3049,13 @@
       <c r="A20" s="43"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F20" s="6">
         <v>0.5</v>
@@ -2989,7 +3064,7 @@
     </row>
     <row r="21" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -3008,13 +3083,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6">
@@ -3026,13 +3101,13 @@
       <c r="A23" s="43"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F23" s="6">
         <v>2</v>
@@ -3043,13 +3118,13 @@
       <c r="A24" s="43"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F24" s="6">
         <v>0.5</v>
@@ -3060,10 +3135,10 @@
       <c r="A25" s="43"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="6">
@@ -3075,10 +3150,10 @@
       <c r="A26" s="43"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="6">
@@ -3090,13 +3165,13 @@
       <c r="A27" s="43"/>
       <c r="B27" s="4"/>
       <c r="C27" s="28" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
@@ -3105,7 +3180,7 @@
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -3124,13 +3199,13 @@
         <v>9</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="6">
@@ -3142,10 +3217,10 @@
       <c r="A30" s="43"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="6">
@@ -3157,13 +3232,13 @@
       <c r="A31" s="43"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F31" s="6">
         <v>2</v>
@@ -3174,13 +3249,13 @@
       <c r="A32" s="43"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F32" s="6">
         <v>1.5</v>
@@ -3191,10 +3266,10 @@
       <c r="A33" s="43"/>
       <c r="B33" s="4"/>
       <c r="C33" s="29" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="29">
@@ -3222,7 +3297,7 @@
     </row>
     <row r="36" spans="1:7" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="19"/>
@@ -3254,7 +3329,7 @@
     </row>
     <row r="38" spans="1:7" s="10" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
@@ -3305,8 +3380,8 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27:F27"/>
+      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3361,7 +3436,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>2</v>
@@ -3388,16 +3463,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F5" s="13">
         <v>4</v>
@@ -3408,13 +3483,13 @@
       <c r="A6" s="43"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F6" s="13">
         <v>0.5</v>
@@ -3425,13 +3500,13 @@
       <c r="A7" s="43"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F7" s="13">
         <v>1.5</v>
@@ -3460,10 +3535,10 @@
       <c r="A10" s="43"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="6">
@@ -3473,7 +3548,7 @@
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -3492,16 +3567,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F12" s="6">
         <v>3.5</v>
@@ -3512,13 +3587,13 @@
       <c r="A13" s="43"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
@@ -3529,13 +3604,13 @@
       <c r="A14" s="43"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F14" s="6">
         <v>1.5</v>
@@ -3546,10 +3621,10 @@
       <c r="A15" s="43"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6">
@@ -3559,7 +3634,7 @@
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -3578,13 +3653,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6">
@@ -3614,10 +3689,10 @@
       <c r="A20" s="43"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="6">
@@ -3627,7 +3702,7 @@
     </row>
     <row r="21" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -3646,16 +3721,16 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F22" s="6">
         <v>3.5</v>
@@ -3666,13 +3741,13 @@
       <c r="A23" s="43"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F23" s="6">
         <v>1.5</v>
@@ -3710,10 +3785,10 @@
       <c r="A27" s="43"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="10">
@@ -3723,7 +3798,7 @@
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -3742,13 +3817,13 @@
         <v>9</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="6">
@@ -3760,10 +3835,10 @@
       <c r="A30" s="43"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="6">
@@ -3775,13 +3850,13 @@
       <c r="A31" s="43"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F31" s="6">
         <v>1.5</v>
@@ -3792,10 +3867,10 @@
       <c r="A32" s="43"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="6">
@@ -3807,13 +3882,13 @@
       <c r="A33" s="43"/>
       <c r="B33" s="4"/>
       <c r="C33" s="29" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F33" s="29">
         <v>1</v>
@@ -3840,7 +3915,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="19"/>
@@ -3872,7 +3947,7 @@
     </row>
     <row r="38" spans="1:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
@@ -3949,8 +4024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF08362A-39DA-4F12-AE49-90700CE33988}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,7 +4075,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>2</v>
@@ -4027,16 +4102,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F5" s="13">
         <v>2</v>
@@ -4047,10 +4122,10 @@
       <c r="A6" s="43"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="29">
@@ -4062,10 +4137,10 @@
       <c r="A7" s="43"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="13">
@@ -4077,13 +4152,13 @@
       <c r="A8" s="43"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F8" s="6">
         <v>1.5</v>
@@ -4110,7 +4185,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -4129,13 +4204,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="29">
@@ -4147,10 +4222,10 @@
       <c r="A13" s="43"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="6">
@@ -4162,10 +4237,10 @@
       <c r="A14" s="43"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6">
@@ -4177,10 +4252,10 @@
       <c r="A15" s="43"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6">
@@ -4190,7 +4265,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -4209,7 +4284,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -4246,7 +4321,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -4265,13 +4340,13 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="29">
@@ -4283,10 +4358,10 @@
       <c r="A23" s="43"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="6">
@@ -4307,10 +4382,10 @@
       <c r="A25" s="43"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="6">
@@ -4338,7 +4413,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -4357,13 +4432,13 @@
         <v>9</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="6">
@@ -4375,10 +4450,10 @@
       <c r="A30" s="43"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="6">
@@ -4390,10 +4465,10 @@
       <c r="A31" s="43"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="29">
@@ -4439,7 +4514,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="19"/>
@@ -4471,7 +4546,7 @@
     </row>
     <row r="38" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
@@ -4514,7 +4589,7 @@
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A22:A27"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5 F7:F11 F13:F21 F36 F23:F26 F28:F30 F32">
+  <conditionalFormatting sqref="F5 F7:F11 F13:F21 F23:F26 F28:F30 F32 F36">
     <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -4539,13 +4614,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33F9F35-91F5-4287-AB11-66F24B7EE014}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:G38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4589,7 +4664,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>2</v>
@@ -4611,24 +4686,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="29">
+        <v>3</v>
+      </c>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4669,7 +4758,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -4679,25 +4768,33 @@
       </c>
       <c r="F11" s="18">
         <f>SUM(F5:F10)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="13">
+        <v>7</v>
+      </c>
       <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
@@ -4723,7 +4820,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -4733,19 +4830,27 @@
       </c>
       <c r="F16" s="18">
         <f>SUM(F12:F15)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="13">
+        <v>7</v>
+      </c>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4770,14 +4875,14 @@
       <c r="A20" s="43"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="10"/>
+      <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -4787,7 +4892,7 @@
       </c>
       <c r="F21" s="18">
         <f>SUM(F17:F20)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G21" s="14"/>
     </row>
@@ -4795,11 +4900,11 @@
       <c r="A22" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4830,44 +4935,42 @@
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="18">
-        <f>SUM(F22:F25)</f>
-        <v>0</v>
-      </c>
+      <c r="A26" s="43"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>9</v>
-      </c>
+      <c r="A27" s="43"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="6"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="18">
+        <f>SUM(F22:F27)</f>
+        <v>0</v>
+      </c>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -4884,108 +4987,108 @@
       <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="43"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="21">
-        <f>SUM(F27:F30)</f>
+      <c r="F36" s="21">
+        <f>SUM(F29:F33)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17" t="s">
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="22">
-        <f>F11+F16+F21+F26+F31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
+      <c r="G37" s="22">
+        <f>F11+F16+F21+F28+F36</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:G38"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A33:G38"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A29:A35"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F31">
+  <conditionalFormatting sqref="F5 F23:F26 F28:F30 F32 F36 F7:F21">
     <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F5)))</formula>
     </cfRule>
@@ -4993,12 +5096,12 @@
       <formula>NOT(ISERROR(SEARCH("En cours",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
+  <conditionalFormatting sqref="G37">
     <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",G32)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",G37)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",G32)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",G37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5140,7 +5243,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -5194,7 +5297,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -5248,7 +5351,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -5302,7 +5405,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -5356,7 +5459,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -5620,7 +5723,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -5674,7 +5777,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -5728,7 +5831,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -5782,7 +5885,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -5836,7 +5939,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -6100,7 +6203,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -6154,7 +6257,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -6208,7 +6311,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -6262,7 +6365,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -6316,7 +6419,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -6576,7 +6679,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -6630,7 +6733,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -6684,7 +6787,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -6738,7 +6841,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -6792,7 +6895,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>

</xml_diff>